<commit_message>
Update toan bo 19 truong ngay_htthucte va sua file excel
</commit_message>
<xml_diff>
--- a/lcnt/static/files/LCNT_file_import - mail.xlsx
+++ b/lcnt/static/files/LCNT_file_import - mail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E82EA9-B330-4897-A0DC-91D233DF90F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6268281-5168-4164-A37C-74B0411E5CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACD26D27-19F9-4437-8E23-6FE16A246B17}"/>
   </bookViews>
@@ -88,17 +88,9 @@
     <t>(11)_Tờ trình phê duyệt Kết quả LCNT</t>
   </si>
   <si>
-    <t>(10)_Hoàn thiện ký biên bản thương thảo
- hợp đồng</t>
-  </si>
-  <si>
     <t>(9)_Thư mời thương thảo</t>
   </si>
   <si>
-    <t>(8)_Ký xong Báo cáo đánh 
-giá của TCG</t>
-  </si>
-  <si>
     <t>(7)_Báo cáo quả_Đánh giá PL-KT-TC</t>
   </si>
   <si>
@@ -169,6 +161,12 @@
   </si>
   <si>
     <t>olympusforce@gmail.com</t>
+  </si>
+  <si>
+    <t>(8)_Ký xong Báo cáo đánh giá của TCG</t>
+  </si>
+  <si>
+    <t>(10)_Hoàn thiện ký biên bản thương thảo hợp đồng</t>
   </si>
 </sst>
 </file>
@@ -396,6 +394,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,9 +412,6 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,9 +423,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -779,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A33B83B-F4B6-41FA-99C4-2C1342E85645}">
   <dimension ref="A1:BM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="BK12" sqref="BK12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,115 +790,115 @@
   <sheetData>
     <row r="1" spans="1:65" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="24" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24" t="s">
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24" t="s">
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24" t="s">
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="25" t="s">
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="20" t="s">
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20" t="s">
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20" t="s">
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20" t="s">
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20" t="s">
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="25" t="s">
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="20" t="s">
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20" t="s">
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="BC1" s="20"/>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="26" t="s">
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="BF1" s="27"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="21" t="s">
+      <c r="BF1" s="28"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="23"/>
+      <c r="BI1" s="24"/>
+      <c r="BJ1" s="25"/>
       <c r="BK1" s="14" t="s">
         <v>7</v>
       </c>
@@ -908,24 +906,24 @@
         <v>6</v>
       </c>
       <c r="BM1" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:65" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>5</v>
@@ -1105,21 +1103,21 @@
         <v>6</v>
       </c>
       <c r="BM2" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:65" ht="102" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1239,10 +1237,10 @@
         <v>45807</v>
       </c>
       <c r="BL3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="BM3" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:65" ht="102" x14ac:dyDescent="0.25">
@@ -1250,13 +1248,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1372,19 +1370,14 @@
         <v>45835</v>
       </c>
       <c r="BL4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="BM4" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
     <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="BH1:BJ1"/>
@@ -1399,6 +1392,11 @@
     <mergeCell ref="AV1:AX1"/>
     <mergeCell ref="AY1:BA1"/>
     <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
@@ -1439,20 +1437,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Them update ngay_htthucte cho 19 step va sua file excel
</commit_message>
<xml_diff>
--- a/lcnt/static/files/LCNT_file_import - mail.xlsx
+++ b/lcnt/static/files/LCNT_file_import - mail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E82EA9-B330-4897-A0DC-91D233DF90F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6268281-5168-4164-A37C-74B0411E5CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACD26D27-19F9-4437-8E23-6FE16A246B17}"/>
   </bookViews>
@@ -88,17 +88,9 @@
     <t>(11)_Tờ trình phê duyệt Kết quả LCNT</t>
   </si>
   <si>
-    <t>(10)_Hoàn thiện ký biên bản thương thảo
- hợp đồng</t>
-  </si>
-  <si>
     <t>(9)_Thư mời thương thảo</t>
   </si>
   <si>
-    <t>(8)_Ký xong Báo cáo đánh 
-giá của TCG</t>
-  </si>
-  <si>
     <t>(7)_Báo cáo quả_Đánh giá PL-KT-TC</t>
   </si>
   <si>
@@ -169,6 +161,12 @@
   </si>
   <si>
     <t>olympusforce@gmail.com</t>
+  </si>
+  <si>
+    <t>(8)_Ký xong Báo cáo đánh giá của TCG</t>
+  </si>
+  <si>
+    <t>(10)_Hoàn thiện ký biên bản thương thảo hợp đồng</t>
   </si>
 </sst>
 </file>
@@ -396,6 +394,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -408,9 +412,6 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,9 +423,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -779,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A33B83B-F4B6-41FA-99C4-2C1342E85645}">
   <dimension ref="A1:BM4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="BK12" sqref="BK12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,115 +790,115 @@
   <sheetData>
     <row r="1" spans="1:65" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="24" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24" t="s">
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24" t="s">
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24" t="s">
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="25" t="s">
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="20" t="s">
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="21"/>
+      <c r="AC1" s="21"/>
+      <c r="AD1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20" t="s">
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="26"/>
+      <c r="AG1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20" t="s">
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20" t="s">
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="22"/>
+      <c r="AP1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20" t="s">
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="25" t="s">
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AW1" s="25"/>
-      <c r="AX1" s="25"/>
-      <c r="AY1" s="20" t="s">
+      <c r="AW1" s="26"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20" t="s">
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="BC1" s="20"/>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="26" t="s">
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="22"/>
+      <c r="BE1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="BF1" s="27"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="21" t="s">
+      <c r="BF1" s="28"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="23"/>
+      <c r="BI1" s="24"/>
+      <c r="BJ1" s="25"/>
       <c r="BK1" s="14" t="s">
         <v>7</v>
       </c>
@@ -908,24 +906,24 @@
         <v>6</v>
       </c>
       <c r="BM1" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:65" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>5</v>
@@ -1105,21 +1103,21 @@
         <v>6</v>
       </c>
       <c r="BM2" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:65" ht="102" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1239,10 +1237,10 @@
         <v>45807</v>
       </c>
       <c r="BL3" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="BM3" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:65" ht="102" x14ac:dyDescent="0.25">
@@ -1250,13 +1248,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1372,19 +1370,14 @@
         <v>45835</v>
       </c>
       <c r="BL4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="BM4" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:T1"/>
     <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="BH1:BJ1"/>
@@ -1399,6 +1392,11 @@
     <mergeCell ref="AV1:AX1"/>
     <mergeCell ref="AY1:BA1"/>
     <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H2">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
@@ -1439,20 +1437,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>